<commit_message>
changes before dinner - 07/11
just getting the measures, code ok!
</commit_message>
<xml_diff>
--- a/TASK_2 - Excel.xlsx
+++ b/TASK_2 - Excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>TASK 2</t>
   </si>
@@ -53,13 +53,70 @@
     <t>Side</t>
   </si>
   <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
-    <t>area</t>
+    <t>med_height</t>
+  </si>
+  <si>
+    <t>med_width</t>
+  </si>
+  <si>
+    <t>max_width</t>
+  </si>
+  <si>
+    <t>max_height</t>
+  </si>
+  <si>
+    <t>area_max</t>
+  </si>
+  <si>
+    <t>631.5</t>
+  </si>
+  <si>
+    <t>579.5</t>
+  </si>
+  <si>
+    <t>611.75</t>
+  </si>
+  <si>
+    <t>553.75</t>
+  </si>
+  <si>
+    <t>592.5</t>
+  </si>
+  <si>
+    <t>1024.5</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>front</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>942.6667</t>
+  </si>
+  <si>
+    <t>773.3333</t>
+  </si>
+  <si>
+    <t>814.6667</t>
+  </si>
+  <si>
+    <t>728.6667</t>
+  </si>
+  <si>
+    <t>916.6667</t>
+  </si>
+  <si>
+    <t>1395.3</t>
+  </si>
+  <si>
+    <t>961.6667</t>
   </si>
 </sst>
 </file>
@@ -148,9 +205,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -158,6 +212,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -442,225 +499,180 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:Q4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="3" t="s">
+      <c r="R2" s="4"/>
+      <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>604</v>
-      </c>
-      <c r="C3" s="1">
-        <v>832</v>
-      </c>
-      <c r="D3" s="1">
-        <v>587</v>
-      </c>
-      <c r="E3" s="1">
-        <v>731</v>
-      </c>
+        <v>683</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
-        <v>564</v>
-      </c>
-      <c r="I3" s="1">
-        <v>720</v>
-      </c>
-      <c r="J3" s="1">
-        <v>578</v>
-      </c>
-      <c r="K3" s="1">
-        <v>658</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1">
-        <v>580</v>
-      </c>
-      <c r="O3" s="1">
-        <v>719</v>
-      </c>
-      <c r="P3" s="1">
-        <v>542</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>775</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1">
-        <v>528</v>
-      </c>
-      <c r="U3" s="1">
-        <v>777</v>
-      </c>
-      <c r="V3" s="1">
-        <v>563</v>
-      </c>
-      <c r="W3" s="1">
-        <v>755</v>
-      </c>
+        <v>670</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>653</v>
-      </c>
-      <c r="C4" s="1">
-        <v>807</v>
-      </c>
-      <c r="D4" s="1">
-        <v>717</v>
-      </c>
-      <c r="E4" s="1">
-        <v>852</v>
-      </c>
+        <v>707</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
-        <v>843</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1232</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1141</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1682</v>
-      </c>
+        <v>644</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1">
-        <v>793</v>
-      </c>
-      <c r="O4" s="1">
-        <v>949</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1081</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1244</v>
-      </c>
+        <v>1281</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1">
-        <v>998</v>
-      </c>
-      <c r="U4" s="1">
-        <v>1409</v>
-      </c>
-      <c r="V4" s="1">
-        <v>907</v>
-      </c>
-      <c r="W4" s="1">
-        <v>900</v>
-      </c>
+        <v>1083</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -711,57 +723,79 @@
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
+      <c r="T7" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>670</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="1">
+        <v>1218</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="T8" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -836,101 +870,172 @@
       <c r="W11" s="1"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>659</v>
+      </c>
+      <c r="C13" s="1">
+        <v>683</v>
+      </c>
+      <c r="D13" s="1">
+        <v>670</v>
+      </c>
+      <c r="E13" s="1">
+        <v>624</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="H13" s="1">
+        <v>838</v>
+      </c>
+      <c r="I13" s="1">
+        <v>949</v>
+      </c>
+      <c r="J13" s="1">
+        <v>868</v>
+      </c>
+      <c r="K13" s="1">
+        <v>770</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>644</v>
+      </c>
+      <c r="C14" s="1">
+        <v>707</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1083</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1281</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="H14" s="1">
+        <v>1089</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1033</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1540</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1607</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -943,94 +1048,122 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="1">
+        <v>889</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1">
+        <v>670</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1218</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>

</xml_diff>

<commit_message>
task 2 done - just need to be cleaned up
</commit_message>
<xml_diff>
--- a/TASK_2 - Excel.xlsx
+++ b/TASK_2 - Excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t>TASK 2</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>area_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -735,7 +732,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+      <selection activeCell="L4" sqref="L4:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +743,7 @@
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="9.140625" style="18"/>
+    <col min="11" max="11" width="13" style="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="1"/>
@@ -933,8 +930,8 @@
       <c r="J5" s="4">
         <v>868</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>39</v>
+      <c r="K5" s="17">
+        <v>770</v>
       </c>
       <c r="L5" s="26"/>
       <c r="M5" s="11" t="s">
@@ -1072,9 +1069,9 @@
         <f t="shared" ref="J7" si="2">J5*2+J6*2</f>
         <v>4816</v>
       </c>
-      <c r="K7" s="17" t="e">
+      <c r="K7" s="17">
         <f t="shared" ref="K7" si="3">K5*2+K6*2</f>
-        <v>#VALUE!</v>
+        <v>4754</v>
       </c>
       <c r="L7" s="26"/>
       <c r="M7" s="11" t="s">
@@ -1154,9 +1151,9 @@
         <f t="shared" si="11"/>
         <v>1336720</v>
       </c>
-      <c r="K8" s="17" t="e">
+      <c r="K8" s="17">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
+        <v>1237390</v>
       </c>
       <c r="L8" s="26"/>
       <c r="M8" s="11" t="s">

</xml_diff>

<commit_message>
relatorio e melhorar decision tree
</commit_message>
<xml_diff>
--- a/TASK_2 - Excel.xlsx
+++ b/TASK_2 - Excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\up201404125\Documents\GitHub\SBVI_Carvana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\Documents\GitHub\SBVI_Carvana\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="50">
   <si>
     <t>TASK 2</t>
   </si>
@@ -141,13 +141,46 @@
   </si>
   <si>
     <t>area_min</t>
+  </si>
+  <si>
+    <t>Relação das alturas (sedan &amp; SUV)</t>
+  </si>
+  <si>
+    <t>Relação das larguras compacto &amp; SUV)</t>
+  </si>
+  <si>
+    <t>Relação das larguras compacto &amp; sedan</t>
+  </si>
+  <si>
+    <t>min_area</t>
+  </si>
+  <si>
+    <t>min_axis</t>
+  </si>
+  <si>
+    <t>min_formula</t>
+  </si>
+  <si>
+    <t>min_box</t>
+  </si>
+  <si>
+    <t>max_area</t>
+  </si>
+  <si>
+    <t>max_axis</t>
+  </si>
+  <si>
+    <t>max_formula</t>
+  </si>
+  <si>
+    <t>max_box</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +192,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -291,15 +338,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -371,11 +409,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,13 +540,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -411,11 +555,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -423,7 +564,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -449,9 +590,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -729,180 +907,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.140625" style="18"/>
+    <col min="5" max="5" width="9.140625" style="16"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="13" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="9.140625" style="18"/>
+    <col min="17" max="17" width="9.140625" style="16"/>
     <col min="18" max="18" width="9.140625" style="1"/>
     <col min="19" max="19" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="9.140625" style="1"/>
-    <col min="23" max="23" width="9.140625" style="18"/>
+    <col min="23" max="23" width="9.140625" style="16"/>
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="18"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="19"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="18"/>
     </row>
     <row r="3" spans="1:24" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="26"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="19"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="18"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="25"/>
+      <c r="G4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="9" t="s">
+      <c r="L4" s="25"/>
+      <c r="M4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="26"/>
-      <c r="S4" s="9" t="s">
+      <c r="R4" s="25"/>
+      <c r="S4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="U4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="17" t="s">
+      <c r="W4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="19"/>
+      <c r="X4" s="18"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4">
@@ -914,11 +1092,11 @@
       <c r="D5" s="4">
         <v>670</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>624</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="25"/>
+      <c r="G5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4">
@@ -930,11 +1108,11 @@
       <c r="J5" s="4">
         <v>868</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="16">
         <v>770</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="11" t="s">
+      <c r="L5" s="25"/>
+      <c r="M5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="N5" s="4">
@@ -946,11 +1124,11 @@
       <c r="P5" s="4">
         <v>606</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="16">
         <v>563</v>
       </c>
-      <c r="R5" s="26"/>
-      <c r="S5" s="11" t="s">
+      <c r="R5" s="25"/>
+      <c r="S5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="T5" s="4">
@@ -962,13 +1140,13 @@
       <c r="V5" s="4">
         <v>775</v>
       </c>
-      <c r="W5" s="17">
+      <c r="W5" s="16">
         <v>658</v>
       </c>
-      <c r="X5" s="19"/>
+      <c r="X5" s="18"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4">
@@ -980,11 +1158,11 @@
       <c r="D6" s="4">
         <v>1083</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>1281</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="25"/>
+      <c r="G6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="4">
@@ -996,11 +1174,11 @@
       <c r="J6" s="4">
         <v>1540</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="16">
         <v>1607</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="11" t="s">
+      <c r="L6" s="25"/>
+      <c r="M6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="N6" s="4">
@@ -1012,11 +1190,11 @@
       <c r="P6" s="4">
         <v>1402</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="16">
         <v>1624</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="11" t="s">
+      <c r="R6" s="25"/>
+      <c r="S6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="T6" s="4">
@@ -1028,13 +1206,13 @@
       <c r="V6" s="4">
         <v>1417</v>
       </c>
-      <c r="W6" s="17">
+      <c r="W6" s="16">
         <v>1706</v>
       </c>
-      <c r="X6" s="19"/>
+      <c r="X6" s="18"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="4">
@@ -1049,12 +1227,12 @@
         <f t="shared" si="0"/>
         <v>3506</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <f t="shared" si="0"/>
         <v>3810</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="4">
@@ -1069,12 +1247,12 @@
         <f t="shared" ref="J7" si="2">J5*2+J6*2</f>
         <v>4816</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="16">
         <f t="shared" ref="K7" si="3">K5*2+K6*2</f>
         <v>4754</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="11" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="N7" s="4">
@@ -1089,12 +1267,12 @@
         <f t="shared" ref="P7" si="5">P5*2+P6*2</f>
         <v>4016</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="16">
         <f t="shared" ref="Q7" si="6">Q5*2+Q6*2</f>
         <v>4374</v>
       </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="11" t="s">
+      <c r="R7" s="25"/>
+      <c r="S7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="T7" s="4">
@@ -1109,14 +1287,14 @@
         <f t="shared" ref="V7" si="8">V5*2+V6*2</f>
         <v>4384</v>
       </c>
-      <c r="W7" s="17">
+      <c r="W7" s="16">
         <f t="shared" ref="W7" si="9">W5*2+W6*2</f>
         <v>4728</v>
       </c>
-      <c r="X7" s="19"/>
+      <c r="X7" s="18"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="4">
@@ -1131,12 +1309,12 @@
         <f t="shared" si="10"/>
         <v>725610</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <f t="shared" si="10"/>
         <v>799344</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="11" t="s">
+      <c r="F8" s="25"/>
+      <c r="G8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="4">
@@ -1151,12 +1329,12 @@
         <f t="shared" si="11"/>
         <v>1336720</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
         <f t="shared" si="11"/>
         <v>1237390</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="11" t="s">
+      <c r="L8" s="25"/>
+      <c r="M8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="N8" s="4">
@@ -1171,12 +1349,12 @@
         <f t="shared" si="12"/>
         <v>849612</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="16">
         <f t="shared" si="12"/>
         <v>914312</v>
       </c>
-      <c r="R8" s="26"/>
-      <c r="S8" s="11" t="s">
+      <c r="R8" s="25"/>
+      <c r="S8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="T8" s="4">
@@ -1191,242 +1369,238 @@
         <f t="shared" si="13"/>
         <v>1098175</v>
       </c>
-      <c r="W8" s="17">
+      <c r="W8" s="16">
         <f t="shared" si="13"/>
         <v>1122548</v>
       </c>
-      <c r="X8" s="19"/>
+      <c r="X8" s="18"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="14"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="14"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="14"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="13"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="19"/>
+      <c r="X9" s="18"/>
     </row>
     <row r="10" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>491</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="11" t="s">
+      <c r="F10" s="25"/>
+      <c r="G10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="17">
+      <c r="K10" s="16">
         <v>662</v>
       </c>
-      <c r="L10" s="26"/>
-      <c r="M10" s="11" t="s">
+      <c r="L10" s="25"/>
+      <c r="M10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="17">
+      <c r="Q10" s="16">
         <v>471</v>
       </c>
-      <c r="R10" s="26"/>
-      <c r="S10" s="11" t="s">
+      <c r="R10" s="25"/>
+      <c r="S10" s="10" t="s">
         <v>35</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
-      <c r="W10" s="17">
+      <c r="W10" s="16">
         <v>592</v>
       </c>
-      <c r="X10" s="19"/>
+      <c r="X10" s="18"/>
     </row>
     <row r="11" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>1174</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="11" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="17">
+      <c r="K11" s="16">
         <v>1279</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="11" t="s">
+      <c r="L11" s="25"/>
+      <c r="M11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="17">
+      <c r="Q11" s="16">
         <v>1338</v>
       </c>
-      <c r="R11" s="26"/>
-      <c r="S11" s="11" t="s">
+      <c r="R11" s="25"/>
+      <c r="S11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
-      <c r="W11" s="17">
+      <c r="W11" s="16">
         <v>1492</v>
       </c>
-      <c r="X11" s="19"/>
+      <c r="X11" s="18"/>
     </row>
     <row r="12" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <f t="shared" ref="E12" si="14">E10*2+E11*2</f>
         <v>3330</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="11" t="s">
+      <c r="F12" s="25"/>
+      <c r="G12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="17">
+      <c r="K12" s="16">
         <f t="shared" ref="K12" si="15">K10*2+K11*2</f>
         <v>3882</v>
       </c>
-      <c r="L12" s="26"/>
-      <c r="M12" s="11" t="s">
+      <c r="L12" s="25"/>
+      <c r="M12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="17">
+      <c r="Q12" s="16">
         <f t="shared" ref="Q12" si="16">Q10*2+Q11*2</f>
         <v>3618</v>
       </c>
-      <c r="R12" s="26"/>
-      <c r="S12" s="11" t="s">
+      <c r="R12" s="25"/>
+      <c r="S12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="17">
+      <c r="W12" s="16">
         <f t="shared" ref="W12" si="17">W10*2+W11*2</f>
         <v>4168</v>
       </c>
-      <c r="X12" s="19"/>
+      <c r="X12" s="18"/>
     </row>
     <row r="13" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <f t="shared" ref="E13" si="18">E10*E11</f>
         <v>576434</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="25"/>
+      <c r="G13" s="10" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="17">
+      <c r="K13" s="16">
         <f t="shared" ref="K13" si="19">K10*K11</f>
         <v>846698</v>
       </c>
-      <c r="L13" s="26"/>
-      <c r="M13" s="11" t="s">
+      <c r="L13" s="25"/>
+      <c r="M13" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="17">
+      <c r="Q13" s="16">
         <f t="shared" ref="Q13" si="20">Q10*Q11</f>
         <v>630198</v>
       </c>
-      <c r="R13" s="26"/>
-      <c r="S13" s="11" t="s">
+      <c r="R13" s="25"/>
+      <c r="S13" s="10" t="s">
         <v>38</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
-      <c r="W13" s="17">
+      <c r="W13" s="16">
         <f t="shared" ref="W13" si="21">W10*W11</f>
         <v>883264</v>
       </c>
-      <c r="X13" s="19"/>
+      <c r="X13" s="18"/>
     </row>
     <row r="14" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="14"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="14"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="13"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="14"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="13"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="19"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="18"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4">
@@ -1438,11 +1612,11 @@
       <c r="D15" s="4">
         <v>592.5</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="16">
         <v>553.75</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="25"/>
+      <c r="G15" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="4">
@@ -1454,11 +1628,11 @@
       <c r="J15" s="4">
         <v>814.66669999999999</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="16">
         <v>728.66669999999999</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="11" t="s">
+      <c r="L15" s="25"/>
+      <c r="M15" s="10" t="s">
         <v>5</v>
       </c>
       <c r="N15" s="4">
@@ -1470,11 +1644,11 @@
       <c r="P15" s="4">
         <v>580.79999999999995</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="16">
         <v>503.2</v>
       </c>
-      <c r="R15" s="26"/>
-      <c r="S15" s="11" t="s">
+      <c r="R15" s="25"/>
+      <c r="S15" s="10" t="s">
         <v>5</v>
       </c>
       <c r="T15" s="4">
@@ -1486,13 +1660,13 @@
       <c r="V15" s="4">
         <v>698.75</v>
       </c>
-      <c r="W15" s="17">
+      <c r="W15" s="16">
         <v>625.25</v>
       </c>
-      <c r="X15" s="19"/>
+      <c r="X15" s="18"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="4">
@@ -1504,11 +1678,11 @@
       <c r="D16" s="4">
         <v>1024.5</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>1218</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="4">
@@ -1520,11 +1694,11 @@
       <c r="J16" s="4">
         <v>1395.3</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="16">
         <v>961.66669999999999</v>
       </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="11" t="s">
+      <c r="L16" s="25"/>
+      <c r="M16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="N16" s="4">
@@ -1536,11 +1710,11 @@
       <c r="P16" s="4">
         <v>1204.2</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="16">
         <v>1497</v>
       </c>
-      <c r="R16" s="26"/>
-      <c r="S16" s="11" t="s">
+      <c r="R16" s="25"/>
+      <c r="S16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="T16" s="4">
@@ -1552,13 +1726,13 @@
       <c r="V16" s="4">
         <v>1319.5</v>
       </c>
-      <c r="W16" s="17">
+      <c r="W16" s="16">
         <v>1587.3</v>
       </c>
-      <c r="X16" s="19"/>
+      <c r="X16" s="18"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4">
@@ -1573,12 +1747,12 @@
         <f t="shared" si="22"/>
         <v>3234</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <f t="shared" si="22"/>
         <v>3543.5</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="25"/>
+      <c r="G17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H17" s="4">
@@ -1593,12 +1767,12 @@
         <f t="shared" ref="J17" si="24">J15*2+J16*2</f>
         <v>4419.9333999999999</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="16">
         <f t="shared" ref="K17" si="25">K15*2+K16*2</f>
         <v>3380.6668</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="11" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="N17" s="4">
@@ -1613,12 +1787,12 @@
         <f t="shared" ref="P17" si="27">P15*2+P16*2</f>
         <v>3570</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="16">
         <f t="shared" ref="Q17" si="28">Q15*2+Q16*2</f>
         <v>4000.4</v>
       </c>
-      <c r="R17" s="26"/>
-      <c r="S17" s="11" t="s">
+      <c r="R17" s="25"/>
+      <c r="S17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="T17" s="4">
@@ -1633,144 +1807,140 @@
         <f t="shared" ref="V17" si="30">V15*2+V16*2</f>
         <v>4036.5</v>
       </c>
-      <c r="W17" s="17">
+      <c r="W17" s="16">
         <f t="shared" ref="W17" si="31">W15*2+W16*2</f>
         <v>4425.1000000000004</v>
       </c>
-      <c r="X17" s="19"/>
+      <c r="X17" s="18"/>
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="12">
         <f>B15*B16</f>
         <v>354509.125</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <f t="shared" ref="C18:E18" si="32">C15*C16</f>
         <v>423105</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <f t="shared" si="32"/>
         <v>607016.25</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <f t="shared" si="32"/>
         <v>674467.5</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="12" t="s">
+      <c r="F18" s="25"/>
+      <c r="G18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="12">
         <f>H15*H16</f>
         <v>728995.54991110996</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="12">
         <f t="shared" ref="I18:K18" si="33">I15*I16</f>
         <v>814916.69629999995</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="12">
         <f t="shared" si="33"/>
         <v>1136704.4465099999</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K18" s="16">
         <f t="shared" si="33"/>
         <v>700734.50078888994</v>
       </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="12" t="s">
+      <c r="L18" s="25"/>
+      <c r="M18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="12">
         <f>N15*N16</f>
         <v>406850.76</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="12">
         <f t="shared" ref="O18:Q18" si="34">O15*O16</f>
         <v>437262.23999999993</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="12">
         <f t="shared" si="34"/>
         <v>699399.36</v>
       </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="16">
         <f t="shared" si="34"/>
         <v>753290.4</v>
       </c>
-      <c r="R18" s="26"/>
-      <c r="S18" s="12" t="s">
+      <c r="R18" s="25"/>
+      <c r="S18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="T18" s="13">
+      <c r="T18" s="12">
         <f>T15*T16</f>
         <v>526079.125</v>
       </c>
-      <c r="U18" s="13">
+      <c r="U18" s="12">
         <f t="shared" ref="U18:W18" si="35">U15*U16</f>
         <v>534838.75</v>
       </c>
-      <c r="V18" s="13">
+      <c r="V18" s="12">
         <f t="shared" si="35"/>
         <v>922000.625</v>
       </c>
-      <c r="W18" s="17">
+      <c r="W18" s="16">
         <f t="shared" si="35"/>
         <v>992459.32499999995</v>
       </c>
-      <c r="X18" s="19"/>
+      <c r="X18" s="18"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="19"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="X19" s="18"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="16" t="s">
         <v>25</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q20" s="17" t="s">
+      <c r="Q20" s="16" t="s">
         <v>23</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W20" s="17">
+      <c r="W20" s="16">
         <v>866</v>
       </c>
     </row>
@@ -1778,25 +1948,25 @@
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="16" t="s">
         <v>26</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="16">
         <v>168</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W21" s="17" t="s">
+      <c r="W21" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1804,25 +1974,25 @@
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="17">
+      <c r="K22" s="16">
         <v>1872</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q22" s="17">
+      <c r="Q22" s="16">
         <v>1665</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W22" s="17" t="s">
+      <c r="W22" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1830,57 +2000,51 @@
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>31</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="16" t="s">
         <v>27</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="Q23" s="16" t="s">
         <v>24</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W23" s="17" t="s">
+      <c r="W23" s="16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="W24" s="17"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="16">
         <v>75</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="17">
+      <c r="K25" s="16">
         <v>187</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q25" s="17">
+      <c r="Q25" s="16">
         <v>75</v>
       </c>
       <c r="S25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W25" s="17">
+      <c r="W25" s="16">
         <v>124</v>
       </c>
     </row>
@@ -1888,30 +2052,291 @@
       <c r="A26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>59</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="17">
+      <c r="K26" s="16">
         <v>136</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="16">
         <v>51</v>
       </c>
       <c r="S26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="W26" s="17">
+      <c r="W26" s="16">
         <v>95</v>
       </c>
     </row>
+    <row r="29" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="16">
+        <v>420298</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="16">
+        <v>548875</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>450796</v>
+      </c>
+      <c r="S29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="W29" s="16">
+        <v>614303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="16">
+        <v>0.38329999999999997</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K30" s="16">
+        <v>0.3931</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q30" s="16">
+        <v>0.31159999999999999</v>
+      </c>
+      <c r="S30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="W30" s="16">
+        <v>0.37940000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="16">
+        <v>23.2623</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K31" s="16">
+        <v>37.735500000000002</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q31" s="16">
+        <v>24.7956</v>
+      </c>
+      <c r="S31" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="W31" s="16">
+        <v>22.673400000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="16">
+        <v>624624</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K32" s="16">
+        <v>1063834</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q32" s="16">
+        <v>630198</v>
+      </c>
+      <c r="S32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="W32" s="16">
+        <v>883264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="W33" s="16"/>
+    </row>
+    <row r="34" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="16">
+        <v>458116</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" s="16">
+        <v>885202</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q34" s="16">
+        <v>584497</v>
+      </c>
+      <c r="S34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="W34" s="16">
+        <v>815131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="16">
+        <v>0.50570000000000004</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q35" s="16">
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="S35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="W35" s="16">
+        <v>0.41549999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="16">
+        <v>25.988900000000001</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" s="16">
+        <v>39.427199999999999</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q36" s="16">
+        <v>28</v>
+      </c>
+      <c r="S36" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="W36" s="16">
+        <v>24.293800000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="16">
+        <v>770016</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K37" s="16">
+        <v>1476860</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q37" s="16">
+        <v>875465</v>
+      </c>
+      <c r="S37" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="W37" s="16">
+        <v>1122548</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="27"/>
+      <c r="Q38" s="27"/>
+    </row>
+    <row r="39" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31">
+        <f>(W11-E6)/W11</f>
+        <v>0.14142091152815014</v>
+      </c>
+      <c r="N39" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="37">
+        <f>(W10-Q5)/W10</f>
+        <v>4.8986486486486486E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="34">
+        <f>(Q11-E6)/Q11</f>
+        <v>4.2600896860986545E-2</v>
+      </c>
+      <c r="Q40" s="28"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E41" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
     <mergeCell ref="X1:X19"/>
     <mergeCell ref="A1:W2"/>
     <mergeCell ref="F4:F18"/>

</xml_diff>

<commit_message>
Tables done, code cleaned
</commit_message>
<xml_diff>
--- a/TASK_2 - Excel.xlsx
+++ b/TASK_2 - Excel.xlsx
@@ -5,14 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\Documents\GitHub\SBVI_Carvana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\up201404125\Documents\GitHub\SBVI_Carvana\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="6030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="6030" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabela1" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabela2" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabela3" sheetId="4" r:id="rId4"/>
+    <sheet name="Tabela4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="76">
   <si>
     <t>TASK 2</t>
   </si>
@@ -391,12 +395,45 @@
   <si>
     <t>Não separa SUV de Compacto</t>
   </si>
+  <si>
+    <t>Pick-Up</t>
+  </si>
+  <si>
+    <t>Compacto</t>
+  </si>
+  <si>
+    <t>Sedan &amp; SUV</t>
+  </si>
+  <si>
+    <t>Compacto &amp; SUV</t>
+  </si>
+  <si>
+    <t>Sedan &amp; Pick-Up</t>
+  </si>
+  <si>
+    <t>SUV &amp; Sedan</t>
+  </si>
+  <si>
+    <t>SUV &amp; Pick-Up</t>
+  </si>
+  <si>
+    <t>Sedan &amp; Compacto</t>
+  </si>
+  <si>
+    <t>Compacto &amp; Sedan</t>
+  </si>
+  <si>
+    <t>Meio termo - Sedan &amp; SUV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,8 +483,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,8 +559,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -864,12 +915,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1008,6 +1216,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1026,94 +1327,85 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1399,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41:R41"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,84 +1716,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="80"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="53"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="84"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="80"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="53"/>
     </row>
     <row r="3" spans="1:24" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="80"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="53"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1519,7 +1811,7 @@
       <c r="E4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87"/>
+      <c r="F4" s="60"/>
       <c r="G4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1535,7 +1827,7 @@
       <c r="K4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="87"/>
+      <c r="L4" s="60"/>
       <c r="M4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1551,7 +1843,7 @@
       <c r="Q4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="87"/>
+      <c r="R4" s="60"/>
       <c r="S4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1859,7 @@
       <c r="W4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="80"/>
+      <c r="X4" s="53"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -1585,7 +1877,7 @@
       <c r="E5" s="41">
         <v>624</v>
       </c>
-      <c r="F5" s="87"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1601,7 +1893,7 @@
       <c r="K5" s="41">
         <v>770</v>
       </c>
-      <c r="L5" s="87"/>
+      <c r="L5" s="60"/>
       <c r="M5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1617,7 +1909,7 @@
       <c r="Q5" s="41">
         <v>563</v>
       </c>
-      <c r="R5" s="87"/>
+      <c r="R5" s="60"/>
       <c r="S5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1633,7 +1925,7 @@
       <c r="W5" s="41">
         <v>658</v>
       </c>
-      <c r="X5" s="80"/>
+      <c r="X5" s="53"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -1651,7 +1943,7 @@
       <c r="E6" s="41">
         <v>1281</v>
       </c>
-      <c r="F6" s="87"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1667,7 +1959,7 @@
       <c r="K6" s="41">
         <v>1607</v>
       </c>
-      <c r="L6" s="87"/>
+      <c r="L6" s="60"/>
       <c r="M6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1683,7 +1975,7 @@
       <c r="Q6" s="41">
         <v>1624</v>
       </c>
-      <c r="R6" s="87"/>
+      <c r="R6" s="60"/>
       <c r="S6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1699,7 +1991,7 @@
       <c r="W6" s="41">
         <v>1706</v>
       </c>
-      <c r="X6" s="80"/>
+      <c r="X6" s="53"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -1721,7 +2013,7 @@
         <f t="shared" si="0"/>
         <v>3810</v>
       </c>
-      <c r="F7" s="87"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="8" t="s">
         <v>14</v>
       </c>
@@ -1741,7 +2033,7 @@
         <f t="shared" ref="K7" si="3">K5*2+K6*2</f>
         <v>4754</v>
       </c>
-      <c r="L7" s="87"/>
+      <c r="L7" s="60"/>
       <c r="M7" s="8" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +2053,7 @@
         <f t="shared" ref="Q7" si="6">Q5*2+Q6*2</f>
         <v>4374</v>
       </c>
-      <c r="R7" s="87"/>
+      <c r="R7" s="60"/>
       <c r="S7" s="8" t="s">
         <v>14</v>
       </c>
@@ -1781,7 +2073,7 @@
         <f t="shared" ref="W7" si="9">W5*2+W6*2</f>
         <v>4728</v>
       </c>
-      <c r="X7" s="80"/>
+      <c r="X7" s="53"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -1803,7 +2095,7 @@
         <f t="shared" si="10"/>
         <v>799344</v>
       </c>
-      <c r="F8" s="87"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1823,7 +2115,7 @@
         <f t="shared" si="11"/>
         <v>1237390</v>
       </c>
-      <c r="L8" s="87"/>
+      <c r="L8" s="60"/>
       <c r="M8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1843,7 +2135,7 @@
         <f t="shared" si="12"/>
         <v>914312</v>
       </c>
-      <c r="R8" s="87"/>
+      <c r="R8" s="60"/>
       <c r="S8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1863,7 +2155,7 @@
         <f t="shared" si="13"/>
         <v>1122548</v>
       </c>
-      <c r="X8" s="80"/>
+      <c r="X8" s="53"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="48"/>
@@ -1871,25 +2163,25 @@
       <c r="C9" s="49"/>
       <c r="D9" s="49"/>
       <c r="E9" s="51"/>
-      <c r="F9" s="87"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="48"/>
       <c r="H9" s="49"/>
       <c r="I9" s="49"/>
       <c r="J9" s="49"/>
       <c r="K9" s="51"/>
-      <c r="L9" s="87"/>
+      <c r="L9" s="60"/>
       <c r="M9" s="48"/>
       <c r="N9" s="49"/>
       <c r="O9" s="49"/>
       <c r="P9" s="49"/>
       <c r="Q9" s="51"/>
-      <c r="R9" s="87"/>
+      <c r="R9" s="60"/>
       <c r="S9" s="48"/>
       <c r="T9" s="49"/>
       <c r="U9" s="49"/>
       <c r="V9" s="49"/>
       <c r="W9" s="51"/>
-      <c r="X9" s="80"/>
+      <c r="X9" s="53"/>
     </row>
     <row r="10" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1901,7 +2193,7 @@
       <c r="E10" s="41">
         <v>491</v>
       </c>
-      <c r="F10" s="87"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="8" t="s">
         <v>35</v>
       </c>
@@ -1911,7 +2203,7 @@
       <c r="K10" s="41">
         <v>662</v>
       </c>
-      <c r="L10" s="87"/>
+      <c r="L10" s="60"/>
       <c r="M10" s="8" t="s">
         <v>35</v>
       </c>
@@ -1921,7 +2213,7 @@
       <c r="Q10" s="41">
         <v>471</v>
       </c>
-      <c r="R10" s="87"/>
+      <c r="R10" s="60"/>
       <c r="S10" s="8" t="s">
         <v>35</v>
       </c>
@@ -1931,7 +2223,7 @@
       <c r="W10" s="41">
         <v>592</v>
       </c>
-      <c r="X10" s="80"/>
+      <c r="X10" s="53"/>
     </row>
     <row r="11" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1943,7 +2235,7 @@
       <c r="E11" s="41">
         <v>1174</v>
       </c>
-      <c r="F11" s="87"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
@@ -1953,7 +2245,7 @@
       <c r="K11" s="41">
         <v>1279</v>
       </c>
-      <c r="L11" s="87"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="8" t="s">
         <v>36</v>
       </c>
@@ -1963,7 +2255,7 @@
       <c r="Q11" s="41">
         <v>1338</v>
       </c>
-      <c r="R11" s="87"/>
+      <c r="R11" s="60"/>
       <c r="S11" s="8" t="s">
         <v>36</v>
       </c>
@@ -1973,7 +2265,7 @@
       <c r="W11" s="41">
         <v>1492</v>
       </c>
-      <c r="X11" s="80"/>
+      <c r="X11" s="53"/>
     </row>
     <row r="12" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -1986,7 +2278,7 @@
         <f t="shared" ref="E12" si="14">E10*2+E11*2</f>
         <v>3330</v>
       </c>
-      <c r="F12" s="87"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="8" t="s">
         <v>37</v>
       </c>
@@ -1997,7 +2289,7 @@
         <f t="shared" ref="K12" si="15">K10*2+K11*2</f>
         <v>3882</v>
       </c>
-      <c r="L12" s="87"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="8" t="s">
         <v>37</v>
       </c>
@@ -2008,7 +2300,7 @@
         <f t="shared" ref="Q12" si="16">Q10*2+Q11*2</f>
         <v>3618</v>
       </c>
-      <c r="R12" s="87"/>
+      <c r="R12" s="60"/>
       <c r="S12" s="8" t="s">
         <v>37</v>
       </c>
@@ -2019,7 +2311,7 @@
         <f t="shared" ref="W12" si="17">W10*2+W11*2</f>
         <v>4168</v>
       </c>
-      <c r="X12" s="80"/>
+      <c r="X12" s="53"/>
     </row>
     <row r="13" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -2032,7 +2324,7 @@
         <f t="shared" ref="E13" si="18">E10*E11</f>
         <v>576434</v>
       </c>
-      <c r="F13" s="87"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
@@ -2043,7 +2335,7 @@
         <f t="shared" ref="K13" si="19">K10*K11</f>
         <v>846698</v>
       </c>
-      <c r="L13" s="87"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="8" t="s">
         <v>38</v>
       </c>
@@ -2054,7 +2346,7 @@
         <f t="shared" ref="Q13" si="20">Q10*Q11</f>
         <v>630198</v>
       </c>
-      <c r="R13" s="87"/>
+      <c r="R13" s="60"/>
       <c r="S13" s="8" t="s">
         <v>38</v>
       </c>
@@ -2065,7 +2357,7 @@
         <f t="shared" ref="W13" si="21">W10*W11</f>
         <v>883264</v>
       </c>
-      <c r="X13" s="80"/>
+      <c r="X13" s="53"/>
     </row>
     <row r="14" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
@@ -2073,25 +2365,25 @@
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
       <c r="E14" s="51"/>
-      <c r="F14" s="87"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="48"/>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
       <c r="J14" s="49"/>
       <c r="K14" s="51"/>
-      <c r="L14" s="87"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="48"/>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
       <c r="P14" s="49"/>
       <c r="Q14" s="51"/>
-      <c r="R14" s="87"/>
+      <c r="R14" s="60"/>
       <c r="S14" s="48"/>
       <c r="T14" s="49"/>
       <c r="U14" s="49"/>
       <c r="V14" s="49"/>
       <c r="W14" s="51"/>
-      <c r="X14" s="80"/>
+      <c r="X14" s="53"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -2109,7 +2401,7 @@
       <c r="E15" s="41">
         <v>553.75</v>
       </c>
-      <c r="F15" s="87"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="8" t="s">
         <v>5</v>
       </c>
@@ -2125,7 +2417,7 @@
       <c r="K15" s="41">
         <v>728.66669999999999</v>
       </c>
-      <c r="L15" s="87"/>
+      <c r="L15" s="60"/>
       <c r="M15" s="8" t="s">
         <v>5</v>
       </c>
@@ -2141,7 +2433,7 @@
       <c r="Q15" s="41">
         <v>503.2</v>
       </c>
-      <c r="R15" s="87"/>
+      <c r="R15" s="60"/>
       <c r="S15" s="8" t="s">
         <v>5</v>
       </c>
@@ -2157,7 +2449,7 @@
       <c r="W15" s="41">
         <v>625.25</v>
       </c>
-      <c r="X15" s="80"/>
+      <c r="X15" s="53"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -2175,7 +2467,7 @@
       <c r="E16" s="41">
         <v>1218</v>
       </c>
-      <c r="F16" s="87"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="8" t="s">
         <v>6</v>
       </c>
@@ -2191,7 +2483,7 @@
       <c r="K16" s="41">
         <v>961.66669999999999</v>
       </c>
-      <c r="L16" s="87"/>
+      <c r="L16" s="60"/>
       <c r="M16" s="8" t="s">
         <v>6</v>
       </c>
@@ -2207,7 +2499,7 @@
       <c r="Q16" s="41">
         <v>1497</v>
       </c>
-      <c r="R16" s="87"/>
+      <c r="R16" s="60"/>
       <c r="S16" s="8" t="s">
         <v>6</v>
       </c>
@@ -2223,7 +2515,7 @@
       <c r="W16" s="41">
         <v>1587.3</v>
       </c>
-      <c r="X16" s="80"/>
+      <c r="X16" s="53"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -2245,7 +2537,7 @@
         <f t="shared" si="22"/>
         <v>3543.5</v>
       </c>
-      <c r="F17" s="87"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2265,7 +2557,7 @@
         <f t="shared" ref="K17" si="25">K15*2+K16*2</f>
         <v>3380.6668</v>
       </c>
-      <c r="L17" s="87"/>
+      <c r="L17" s="60"/>
       <c r="M17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2285,7 +2577,7 @@
         <f t="shared" ref="Q17" si="28">Q15*2+Q16*2</f>
         <v>4000.4</v>
       </c>
-      <c r="R17" s="87"/>
+      <c r="R17" s="60"/>
       <c r="S17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2305,7 +2597,7 @@
         <f t="shared" ref="W17" si="31">W15*2+W16*2</f>
         <v>4425.1000000000004</v>
       </c>
-      <c r="X17" s="80"/>
+      <c r="X17" s="53"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -2327,7 +2619,7 @@
         <f t="shared" si="32"/>
         <v>674467.5</v>
       </c>
-      <c r="F18" s="87"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="8" t="s">
         <v>34</v>
       </c>
@@ -2347,7 +2639,7 @@
         <f t="shared" si="33"/>
         <v>700734.50078888994</v>
       </c>
-      <c r="L18" s="87"/>
+      <c r="L18" s="60"/>
       <c r="M18" s="8" t="s">
         <v>34</v>
       </c>
@@ -2367,7 +2659,7 @@
         <f t="shared" si="34"/>
         <v>753290.4</v>
       </c>
-      <c r="R18" s="87"/>
+      <c r="R18" s="60"/>
       <c r="S18" s="8" t="s">
         <v>34</v>
       </c>
@@ -2387,7 +2679,7 @@
         <f t="shared" si="35"/>
         <v>992459.32499999995</v>
       </c>
-      <c r="X18" s="80"/>
+      <c r="X18" s="53"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
@@ -2413,7 +2705,7 @@
       <c r="U19" s="46"/>
       <c r="V19" s="46"/>
       <c r="W19" s="51"/>
-      <c r="X19" s="80"/>
+      <c r="X19" s="53"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -2848,101 +3140,101 @@
         <v>1122548</v>
       </c>
     </row>
-    <row r="37" spans="1:24" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:24" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:24" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="78"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="78"/>
-      <c r="K39" s="78"/>
-      <c r="L39" s="78"/>
-      <c r="M39" s="78"/>
-      <c r="N39" s="78"/>
-      <c r="O39" s="78"/>
-      <c r="P39" s="78"/>
-      <c r="Q39" s="78"/>
-      <c r="R39" s="78"/>
-      <c r="S39" s="78"/>
-      <c r="T39" s="78"/>
-      <c r="U39" s="78"/>
-      <c r="V39" s="78"/>
-      <c r="W39" s="78"/>
-      <c r="X39" s="78"/>
+    <row r="37" spans="1:24" s="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:24" s="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:24" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="61"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="61"/>
+      <c r="P39" s="61"/>
+      <c r="Q39" s="61"/>
+      <c r="R39" s="61"/>
+      <c r="S39" s="61"/>
+      <c r="T39" s="61"/>
+      <c r="U39" s="61"/>
+      <c r="V39" s="61"/>
+      <c r="W39" s="61"/>
+      <c r="X39" s="61"/>
     </row>
     <row r="40" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
+      <c r="A40" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="61"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
       <c r="G40" s="19"/>
-      <c r="H40" s="61" t="s">
+      <c r="H40" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="63"/>
       <c r="N40" s="19"/>
-      <c r="O40" s="61" t="s">
+      <c r="O40" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="P40" s="61"/>
-      <c r="Q40" s="61"/>
-      <c r="R40" s="61"/>
-      <c r="S40" s="61"/>
-      <c r="T40" s="61"/>
+      <c r="P40" s="63"/>
+      <c r="Q40" s="63"/>
+      <c r="R40" s="63"/>
+      <c r="S40" s="63"/>
+      <c r="T40" s="63"/>
       <c r="U40" s="20"/>
     </row>
     <row r="41" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="60" t="s">
+      <c r="A41" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="58">
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="64">
         <f>(W10-Q5)/W10</f>
         <v>4.8986486486486486E-2</v>
       </c>
-      <c r="F41" s="58"/>
+      <c r="F41" s="64"/>
       <c r="G41" s="32">
         <v>3</v>
       </c>
-      <c r="H41" s="60" t="s">
+      <c r="H41" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="60"/>
-      <c r="L41" s="58">
+      <c r="I41" s="65"/>
+      <c r="J41" s="65"/>
+      <c r="K41" s="65"/>
+      <c r="L41" s="64">
         <f>(W31-E36)/W31</f>
         <v>0.12821534671400622</v>
       </c>
-      <c r="M41" s="58"/>
+      <c r="M41" s="64"/>
       <c r="N41" s="25"/>
-      <c r="O41" s="62" t="s">
+      <c r="O41" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="P41" s="62"/>
-      <c r="Q41" s="62"/>
-      <c r="R41" s="62"/>
-      <c r="S41" s="63">
+      <c r="P41" s="81"/>
+      <c r="Q41" s="81"/>
+      <c r="R41" s="81"/>
+      <c r="S41" s="82">
         <f>(K30-Q35)/K30</f>
         <v>0.25799313643651206</v>
       </c>
-      <c r="T41" s="63"/>
+      <c r="T41" s="82"/>
       <c r="U41" s="27">
         <v>1</v>
       </c>
@@ -2954,202 +3246,202 @@
       </c>
     </row>
     <row r="42" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="58">
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="64">
         <f>(K10-Q5)/K10</f>
         <v>0.14954682779456194</v>
       </c>
-      <c r="F42" s="58"/>
+      <c r="F42" s="64"/>
       <c r="G42" s="25"/>
-      <c r="H42" s="60" t="s">
+      <c r="H42" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="60"/>
-      <c r="L42" s="58">
+      <c r="I42" s="65"/>
+      <c r="J42" s="65"/>
+      <c r="K42" s="65"/>
+      <c r="L42" s="64">
         <f>(W31-Q36)/W31</f>
         <v>8.8297496558220421E-3</v>
       </c>
-      <c r="M42" s="58"/>
+      <c r="M42" s="64"/>
       <c r="N42" s="29">
         <v>1</v>
       </c>
-      <c r="O42" s="60" t="s">
+      <c r="O42" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="P42" s="60"/>
-      <c r="Q42" s="60"/>
-      <c r="R42" s="60"/>
-      <c r="S42" s="58">
+      <c r="P42" s="65"/>
+      <c r="Q42" s="65"/>
+      <c r="R42" s="65"/>
+      <c r="S42" s="64">
         <f>(Q30-W35)/Q30</f>
         <v>2.0237461485102168E-2</v>
       </c>
-      <c r="T42" s="58"/>
+      <c r="T42" s="64"/>
       <c r="U42" s="24"/>
     </row>
     <row r="43" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="58">
+      <c r="B43" s="65"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="64">
         <f>(K10-W5)/K10</f>
         <v>6.0422960725075529E-3</v>
       </c>
-      <c r="F43" s="58"/>
+      <c r="F43" s="64"/>
       <c r="G43" s="25"/>
-      <c r="H43" s="60" t="s">
+      <c r="H43" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="I43" s="60"/>
-      <c r="J43" s="60"/>
-      <c r="K43" s="60"/>
-      <c r="L43" s="58">
+      <c r="I43" s="65"/>
+      <c r="J43" s="65"/>
+      <c r="K43" s="65"/>
+      <c r="L43" s="64">
         <f>(K31-Q36)/K31</f>
         <v>0.17706615881801108</v>
       </c>
-      <c r="M43" s="58"/>
+      <c r="M43" s="64"/>
       <c r="N43" s="25"/>
-      <c r="O43" s="60" t="s">
+      <c r="O43" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="P43" s="60"/>
-      <c r="Q43" s="60"/>
-      <c r="R43" s="60"/>
-      <c r="S43" s="58">
+      <c r="P43" s="65"/>
+      <c r="Q43" s="65"/>
+      <c r="R43" s="65"/>
+      <c r="S43" s="64">
         <f>(K30-W35)/K30</f>
         <v>0.35620834492719056</v>
       </c>
-      <c r="T43" s="58"/>
+      <c r="T43" s="64"/>
       <c r="U43" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="59"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="60"/>
-      <c r="J44" s="60"/>
-      <c r="K44" s="60"/>
-      <c r="L44" s="58"/>
-      <c r="M44" s="58"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
       <c r="N44" s="25"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="59"/>
-      <c r="Q44" s="59"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="58"/>
+      <c r="O44" s="69"/>
+      <c r="P44" s="69"/>
+      <c r="Q44" s="69"/>
+      <c r="R44" s="69"/>
+      <c r="S44" s="64"/>
+      <c r="T44" s="64"/>
       <c r="U44" s="24"/>
     </row>
-    <row r="45" spans="1:24" s="71" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="72"/>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="73"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="73"/>
-      <c r="L45" s="73"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="73"/>
-      <c r="P45" s="73"/>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73"/>
-      <c r="T45" s="73"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="74"/>
-      <c r="W45" s="74"/>
-      <c r="X45" s="74"/>
+    <row r="45" spans="1:24" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="77"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="78"/>
+      <c r="J45" s="78"/>
+      <c r="K45" s="78"/>
+      <c r="L45" s="78"/>
+      <c r="M45" s="78"/>
+      <c r="N45" s="79"/>
+      <c r="O45" s="78"/>
+      <c r="P45" s="78"/>
+      <c r="Q45" s="78"/>
+      <c r="R45" s="78"/>
+      <c r="S45" s="78"/>
+      <c r="T45" s="78"/>
+      <c r="U45" s="79"/>
+      <c r="V45" s="79"/>
+      <c r="W45" s="79"/>
+      <c r="X45" s="79"/>
     </row>
     <row r="46" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="61" t="s">
+      <c r="A46" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
       <c r="G46" s="22"/>
-      <c r="H46" s="61" t="s">
+      <c r="H46" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="63"/>
       <c r="N46" s="22"/>
-      <c r="O46" s="61" t="s">
+      <c r="O46" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="P46" s="61"/>
-      <c r="Q46" s="61"/>
-      <c r="R46" s="61"/>
-      <c r="S46" s="61"/>
-      <c r="T46" s="61"/>
+      <c r="P46" s="63"/>
+      <c r="Q46" s="63"/>
+      <c r="R46" s="63"/>
+      <c r="S46" s="63"/>
+      <c r="T46" s="63"/>
       <c r="U46" s="23"/>
     </row>
     <row r="47" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="60" t="s">
+      <c r="A47" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="58">
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="64">
         <f>(W11-E6)/W11</f>
         <v>0.14142091152815014</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="H47" s="60" t="s">
+      <c r="F47" s="64"/>
+      <c r="H47" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="58">
+      <c r="I47" s="65"/>
+      <c r="J47" s="65"/>
+      <c r="K47" s="65"/>
+      <c r="L47" s="64">
         <f>(W28-E33)/W28</f>
         <v>0.25425075247882561</v>
       </c>
-      <c r="M47" s="58"/>
+      <c r="M47" s="64"/>
       <c r="N47" s="31">
         <v>3</v>
       </c>
-      <c r="O47" s="60" t="s">
+      <c r="O47" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="60"/>
-      <c r="R47" s="60"/>
-      <c r="S47" s="58">
+      <c r="P47" s="65"/>
+      <c r="Q47" s="65"/>
+      <c r="R47" s="65"/>
+      <c r="S47" s="64">
         <f>(E29-Q34)/E29</f>
         <v>5.5309157318027651E-2</v>
       </c>
-      <c r="T47" s="58"/>
+      <c r="T47" s="64"/>
       <c r="U47" s="27">
         <v>3</v>
       </c>
@@ -3161,117 +3453,117 @@
       </c>
     </row>
     <row r="48" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="60" t="s">
+      <c r="A48" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="58">
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="64">
         <f>(Q11-E6)/Q11</f>
         <v>4.2600896860986545E-2</v>
       </c>
-      <c r="F48" s="58"/>
+      <c r="F48" s="64"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="60" t="s">
+      <c r="H48" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="I48" s="60"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="60"/>
-      <c r="L48" s="58">
+      <c r="I48" s="65"/>
+      <c r="J48" s="65"/>
+      <c r="K48" s="65"/>
+      <c r="L48" s="64">
         <f>(W28-Q33)/W28</f>
         <v>4.8520030017759966E-2</v>
       </c>
-      <c r="M48" s="58"/>
+      <c r="M48" s="64"/>
       <c r="N48" s="28">
         <v>2</v>
       </c>
-      <c r="O48" s="60" t="s">
+      <c r="O48" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="P48" s="60"/>
-      <c r="Q48" s="60"/>
-      <c r="R48" s="60"/>
-      <c r="S48" s="58">
+      <c r="P48" s="65"/>
+      <c r="Q48" s="65"/>
+      <c r="R48" s="65"/>
+      <c r="S48" s="64">
         <f>(W29-Q34)/W29</f>
         <v>4.5598313125988499E-2</v>
       </c>
-      <c r="T48" s="58"/>
+      <c r="T48" s="64"/>
       <c r="U48" s="24"/>
       <c r="W48" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="59" t="s">
+      <c r="A49" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="68"/>
-      <c r="H49" s="59" t="s">
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="74"/>
+      <c r="H49" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="I49" s="59"/>
-      <c r="J49" s="59"/>
-      <c r="K49" s="59"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="58"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="69"/>
+      <c r="K49" s="69"/>
+      <c r="L49" s="64"/>
+      <c r="M49" s="64"/>
       <c r="N49" s="21"/>
-      <c r="O49" s="60" t="s">
+      <c r="O49" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="P49" s="60"/>
-      <c r="Q49" s="60"/>
-      <c r="R49" s="60"/>
-      <c r="S49" s="58">
+      <c r="P49" s="65"/>
+      <c r="Q49" s="65"/>
+      <c r="R49" s="65"/>
+      <c r="S49" s="64">
         <f>(K29-Q34)/K29</f>
         <v>7.8860340880183233E-2</v>
       </c>
-      <c r="T49" s="58"/>
+      <c r="T49" s="64"/>
       <c r="U49" s="24"/>
     </row>
     <row r="50" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="75"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="70"/>
-      <c r="H50" s="59" t="s">
+      <c r="A50" s="66"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="76"/>
+      <c r="H50" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="I50" s="59"/>
-      <c r="J50" s="59"/>
-      <c r="K50" s="59"/>
-      <c r="O50" s="59" t="s">
+      <c r="I50" s="69"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
+      <c r="O50" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="P50" s="59"/>
-      <c r="Q50" s="59"/>
-      <c r="R50" s="59"/>
-      <c r="S50" s="58"/>
-      <c r="T50" s="58"/>
+      <c r="P50" s="69"/>
+      <c r="Q50" s="69"/>
+      <c r="R50" s="69"/>
+      <c r="S50" s="64"/>
+      <c r="T50" s="64"/>
     </row>
     <row r="51" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="64"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="66"/>
-      <c r="H51" s="60" t="s">
+      <c r="A51" s="70"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="72"/>
+      <c r="H51" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="I51" s="60"/>
-      <c r="J51" s="60"/>
-      <c r="K51" s="60"/>
-      <c r="L51" s="58">
+      <c r="I51" s="65"/>
+      <c r="J51" s="65"/>
+      <c r="K51" s="65"/>
+      <c r="L51" s="64">
         <f>(W28-(Q33+Q28)/2)/W28</f>
         <v>0.15734336312861893</v>
       </c>
-      <c r="M51" s="58"/>
+      <c r="M51" s="64"/>
       <c r="N51" s="32">
         <v>2</v>
       </c>
@@ -3293,34 +3585,34 @@
       </c>
     </row>
     <row r="52" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="64"/>
-      <c r="B52" s="65"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="66"/>
-    </row>
-    <row r="53" spans="1:23" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="53"/>
-      <c r="M53" s="53"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="53"/>
-      <c r="R53" s="53"/>
-      <c r="S53" s="53"/>
-      <c r="T53" s="53"/>
-      <c r="U53" s="53"/>
-      <c r="V53" s="53"/>
-      <c r="W53" s="53"/>
+      <c r="A52" s="70"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72"/>
+    </row>
+    <row r="53" spans="1:23" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="84"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="84"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="84"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="84"/>
+      <c r="N53" s="84"/>
+      <c r="O53" s="84"/>
+      <c r="P53" s="84"/>
+      <c r="Q53" s="84"/>
+      <c r="R53" s="84"/>
+      <c r="S53" s="84"/>
+      <c r="T53" s="84"/>
+      <c r="U53" s="84"/>
+      <c r="V53" s="84"/>
+      <c r="W53" s="84"/>
     </row>
     <row r="54" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E54" s="39"/>
@@ -3438,57 +3730,6 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="X1:X19"/>
-    <mergeCell ref="A1:W2"/>
-    <mergeCell ref="F4:F18"/>
-    <mergeCell ref="L4:L18"/>
-    <mergeCell ref="R4:R18"/>
-    <mergeCell ref="A39:XFD39"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="H40:M40"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="O43:R43"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="A45:XFD45"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="O50:R50"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="H46:M46"/>
-    <mergeCell ref="O40:T40"/>
-    <mergeCell ref="O46:T46"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="O41:R41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="O42:R42"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="L49:M49"/>
     <mergeCell ref="A53:XFD53"/>
     <mergeCell ref="A37:XFD38"/>
     <mergeCell ref="A3:W3"/>
@@ -3505,6 +3746,57 @@
     <mergeCell ref="O49:R49"/>
     <mergeCell ref="S49:T49"/>
     <mergeCell ref="H47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="A45:XFD45"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="O50:R50"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="H46:M46"/>
+    <mergeCell ref="O46:T46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A39:XFD39"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="H40:M40"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="O43:R43"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="O40:T40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="O41:R41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="O42:R42"/>
+    <mergeCell ref="X1:X19"/>
+    <mergeCell ref="A1:W2"/>
+    <mergeCell ref="F4:F18"/>
+    <mergeCell ref="L4:L18"/>
+    <mergeCell ref="R4:R18"/>
   </mergeCells>
   <conditionalFormatting sqref="E47:F48 E41:F43 L41:M43 S41:T43 S47:T49">
     <cfRule type="colorScale" priority="15">
@@ -3689,4 +3981,1630 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:V28"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" s="98" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="113" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="115" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="112" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="113" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="92">
+        <v>659</v>
+      </c>
+      <c r="D3" s="92">
+        <v>683</v>
+      </c>
+      <c r="E3" s="92">
+        <v>670</v>
+      </c>
+      <c r="F3" s="93">
+        <v>624</v>
+      </c>
+      <c r="H3" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="92">
+        <v>590</v>
+      </c>
+      <c r="J3" s="92">
+        <v>630</v>
+      </c>
+      <c r="K3" s="92">
+        <v>606</v>
+      </c>
+      <c r="L3" s="93">
+        <v>563</v>
+      </c>
+      <c r="V3" s="91"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="94">
+        <v>579.5</v>
+      </c>
+      <c r="D4" s="94">
+        <v>631.5</v>
+      </c>
+      <c r="E4" s="94">
+        <v>592.5</v>
+      </c>
+      <c r="F4" s="95">
+        <v>553.75</v>
+      </c>
+      <c r="H4" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="94">
+        <v>564.6</v>
+      </c>
+      <c r="J4" s="94">
+        <v>600.79999999999995</v>
+      </c>
+      <c r="K4" s="94">
+        <v>580.79999999999995</v>
+      </c>
+      <c r="L4" s="95">
+        <v>503.2</v>
+      </c>
+      <c r="V4" s="91"/>
+    </row>
+    <row r="5" spans="2:22" s="91" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="96">
+        <v>487</v>
+      </c>
+      <c r="D5" s="96">
+        <v>577</v>
+      </c>
+      <c r="E5" s="96">
+        <v>508</v>
+      </c>
+      <c r="F5" s="97">
+        <v>491</v>
+      </c>
+      <c r="H5" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="96">
+        <v>542</v>
+      </c>
+      <c r="J5" s="96">
+        <v>565</v>
+      </c>
+      <c r="K5" s="96">
+        <v>563</v>
+      </c>
+      <c r="L5" s="97">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="92">
+        <v>644</v>
+      </c>
+      <c r="D6" s="92">
+        <v>707</v>
+      </c>
+      <c r="E6" s="92">
+        <v>1083</v>
+      </c>
+      <c r="F6" s="93">
+        <v>1281</v>
+      </c>
+      <c r="H6" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="92">
+        <v>758</v>
+      </c>
+      <c r="J6" s="92">
+        <v>787</v>
+      </c>
+      <c r="K6" s="92">
+        <v>1402</v>
+      </c>
+      <c r="L6" s="93">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="94">
+        <v>611.75</v>
+      </c>
+      <c r="D7" s="94">
+        <v>670</v>
+      </c>
+      <c r="E7" s="94">
+        <v>1024.5</v>
+      </c>
+      <c r="F7" s="95">
+        <v>1218</v>
+      </c>
+      <c r="H7" s="100" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="94">
+        <v>720.6</v>
+      </c>
+      <c r="J7" s="94">
+        <v>727.8</v>
+      </c>
+      <c r="K7" s="94">
+        <v>1204.2</v>
+      </c>
+      <c r="L7" s="95">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" s="91" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="96">
+        <v>593</v>
+      </c>
+      <c r="D8" s="96">
+        <v>641</v>
+      </c>
+      <c r="E8" s="96">
+        <v>968</v>
+      </c>
+      <c r="F8" s="97">
+        <v>1174</v>
+      </c>
+      <c r="H8" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="96">
+        <v>672</v>
+      </c>
+      <c r="J8" s="96">
+        <v>660</v>
+      </c>
+      <c r="K8" s="96">
+        <v>1031</v>
+      </c>
+      <c r="L8" s="97">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="92">
+        <f>C3*2+C6*2</f>
+        <v>2606</v>
+      </c>
+      <c r="D9" s="92">
+        <f t="shared" ref="D9:U9" si="0">D3*2+D6*2</f>
+        <v>2780</v>
+      </c>
+      <c r="E9" s="92">
+        <f t="shared" si="0"/>
+        <v>3506</v>
+      </c>
+      <c r="F9" s="93">
+        <f t="shared" si="0"/>
+        <v>3810</v>
+      </c>
+      <c r="H9" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="92">
+        <f>I3*2+I6*2</f>
+        <v>2696</v>
+      </c>
+      <c r="J9" s="92">
+        <f>J3*2+J6*2</f>
+        <v>2834</v>
+      </c>
+      <c r="K9" s="92">
+        <f>K3*2+K6*2</f>
+        <v>4016</v>
+      </c>
+      <c r="L9" s="93">
+        <f>L3*2+L6*2</f>
+        <v>4374</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="94">
+        <f>C7*2+C4*2</f>
+        <v>2382.5</v>
+      </c>
+      <c r="D10" s="94">
+        <f t="shared" ref="D10:F10" si="1">D7*2+D4*2</f>
+        <v>2603</v>
+      </c>
+      <c r="E10" s="94">
+        <f t="shared" si="1"/>
+        <v>3234</v>
+      </c>
+      <c r="F10" s="95">
+        <f t="shared" si="1"/>
+        <v>3543.5</v>
+      </c>
+      <c r="H10" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="94">
+        <f t="shared" ref="I10:L10" si="2">I4*2+I7*2</f>
+        <v>2570.4</v>
+      </c>
+      <c r="J10" s="94">
+        <f t="shared" si="2"/>
+        <v>2657.2</v>
+      </c>
+      <c r="K10" s="94">
+        <f t="shared" si="2"/>
+        <v>3570</v>
+      </c>
+      <c r="L10" s="95">
+        <f t="shared" si="2"/>
+        <v>4000.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" s="91" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="96">
+        <f>C8*2+C5*2</f>
+        <v>2160</v>
+      </c>
+      <c r="D11" s="96">
+        <f t="shared" ref="D11:F11" si="3">D8*2+D5*2</f>
+        <v>2436</v>
+      </c>
+      <c r="E11" s="96">
+        <f t="shared" si="3"/>
+        <v>2952</v>
+      </c>
+      <c r="F11" s="97">
+        <f t="shared" si="3"/>
+        <v>3330</v>
+      </c>
+      <c r="H11" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="96">
+        <f t="shared" ref="I11:L11" si="4">I5*2+I8*2</f>
+        <v>2428</v>
+      </c>
+      <c r="J11" s="96">
+        <f t="shared" si="4"/>
+        <v>2450</v>
+      </c>
+      <c r="K11" s="96">
+        <f t="shared" si="4"/>
+        <v>3188</v>
+      </c>
+      <c r="L11" s="97">
+        <f t="shared" si="4"/>
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="92">
+        <f>C6*C3</f>
+        <v>424396</v>
+      </c>
+      <c r="D12" s="92">
+        <f t="shared" ref="D12:F12" si="5">D6*D3</f>
+        <v>482881</v>
+      </c>
+      <c r="E12" s="92">
+        <f t="shared" si="5"/>
+        <v>725610</v>
+      </c>
+      <c r="F12" s="93">
+        <f t="shared" si="5"/>
+        <v>799344</v>
+      </c>
+      <c r="H12" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="92">
+        <f>I6*I3</f>
+        <v>447220</v>
+      </c>
+      <c r="J12" s="92">
+        <f>J6*J3</f>
+        <v>495810</v>
+      </c>
+      <c r="K12" s="92">
+        <f>K6*K3</f>
+        <v>849612</v>
+      </c>
+      <c r="L12" s="93">
+        <f>L6*L3</f>
+        <v>914312</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="94">
+        <f>C7*C4</f>
+        <v>354509.125</v>
+      </c>
+      <c r="D13" s="94">
+        <f t="shared" ref="D13:F13" si="6">D7*D4</f>
+        <v>423105</v>
+      </c>
+      <c r="E13" s="94">
+        <f t="shared" si="6"/>
+        <v>607016.25</v>
+      </c>
+      <c r="F13" s="95">
+        <f t="shared" si="6"/>
+        <v>674467.5</v>
+      </c>
+      <c r="H13" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="94">
+        <f>I7*I4</f>
+        <v>406850.76</v>
+      </c>
+      <c r="J13" s="94">
+        <f>J7*J4</f>
+        <v>437262.23999999993</v>
+      </c>
+      <c r="K13" s="94">
+        <f>K7*K4</f>
+        <v>699399.36</v>
+      </c>
+      <c r="L13" s="95">
+        <f>L7*L4</f>
+        <v>753290.4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="96">
+        <f t="shared" ref="C14:F14" si="7">C8*C5</f>
+        <v>288791</v>
+      </c>
+      <c r="D14" s="96">
+        <f t="shared" si="7"/>
+        <v>369857</v>
+      </c>
+      <c r="E14" s="96">
+        <f t="shared" si="7"/>
+        <v>491744</v>
+      </c>
+      <c r="F14" s="97">
+        <f t="shared" si="7"/>
+        <v>576434</v>
+      </c>
+      <c r="H14" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="96">
+        <f>I8*I5</f>
+        <v>364224</v>
+      </c>
+      <c r="J14" s="96">
+        <f>J8*J5</f>
+        <v>372900</v>
+      </c>
+      <c r="K14" s="96">
+        <f>K8*K5</f>
+        <v>580453</v>
+      </c>
+      <c r="L14" s="97">
+        <f>L8*L5</f>
+        <v>630198</v>
+      </c>
+      <c r="V14" s="91"/>
+    </row>
+    <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="112" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="113" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="115" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="113" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="113" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="114" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="92">
+        <v>838</v>
+      </c>
+      <c r="D17" s="92">
+        <v>949</v>
+      </c>
+      <c r="E17" s="92">
+        <v>868</v>
+      </c>
+      <c r="F17" s="93">
+        <v>770</v>
+      </c>
+      <c r="H17" s="99" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="92">
+        <v>755</v>
+      </c>
+      <c r="J17" s="92">
+        <v>731</v>
+      </c>
+      <c r="K17" s="92">
+        <v>775</v>
+      </c>
+      <c r="L17" s="93">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="94">
+        <v>773.33330000000001</v>
+      </c>
+      <c r="D18" s="94">
+        <v>889</v>
+      </c>
+      <c r="E18" s="94">
+        <v>814.66669999999999</v>
+      </c>
+      <c r="F18" s="95">
+        <v>728.66669999999999</v>
+      </c>
+      <c r="H18" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="94">
+        <v>679.25</v>
+      </c>
+      <c r="J18" s="94">
+        <v>683.5</v>
+      </c>
+      <c r="K18" s="94">
+        <v>698.75</v>
+      </c>
+      <c r="L18" s="95">
+        <v>625.25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="96">
+        <v>669</v>
+      </c>
+      <c r="D19" s="96">
+        <v>779</v>
+      </c>
+      <c r="E19" s="96">
+        <v>722</v>
+      </c>
+      <c r="F19" s="97">
+        <v>662</v>
+      </c>
+      <c r="H19" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="96">
+        <v>613</v>
+      </c>
+      <c r="J19" s="96">
+        <v>651</v>
+      </c>
+      <c r="K19" s="96">
+        <v>636</v>
+      </c>
+      <c r="L19" s="97">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="92">
+        <v>1089</v>
+      </c>
+      <c r="D20" s="92">
+        <v>1033</v>
+      </c>
+      <c r="E20" s="92">
+        <v>1540</v>
+      </c>
+      <c r="F20" s="93">
+        <v>1607</v>
+      </c>
+      <c r="H20" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="92">
+        <v>872</v>
+      </c>
+      <c r="J20" s="92">
+        <v>852</v>
+      </c>
+      <c r="K20" s="92">
+        <v>1417</v>
+      </c>
+      <c r="L20" s="93">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="94">
+        <v>942.66669999999999</v>
+      </c>
+      <c r="D21" s="94">
+        <v>916.66669999999999</v>
+      </c>
+      <c r="E21" s="94">
+        <v>1395.3</v>
+      </c>
+      <c r="F21" s="95">
+        <v>961.66669999999999</v>
+      </c>
+      <c r="H21" s="100" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="94">
+        <v>774.5</v>
+      </c>
+      <c r="J21" s="94">
+        <v>782.5</v>
+      </c>
+      <c r="K21" s="94">
+        <v>1319.5</v>
+      </c>
+      <c r="L21" s="95">
+        <v>1587.3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="96">
+        <v>780</v>
+      </c>
+      <c r="D22" s="96">
+        <v>741</v>
+      </c>
+      <c r="E22" s="96">
+        <v>1294</v>
+      </c>
+      <c r="F22" s="97">
+        <v>1279</v>
+      </c>
+      <c r="H22" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="96">
+        <v>694</v>
+      </c>
+      <c r="J22" s="96">
+        <v>732</v>
+      </c>
+      <c r="K22" s="96">
+        <v>1284</v>
+      </c>
+      <c r="L22" s="97">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="92">
+        <f>C17*2+C20*2</f>
+        <v>3854</v>
+      </c>
+      <c r="D23" s="92">
+        <f>D17*2+D20*2</f>
+        <v>3964</v>
+      </c>
+      <c r="E23" s="92">
+        <f>E17*2+E20*2</f>
+        <v>4816</v>
+      </c>
+      <c r="F23" s="93">
+        <f>F17*2+F20*2</f>
+        <v>4754</v>
+      </c>
+      <c r="H23" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="92">
+        <f>I17*2+I20*2</f>
+        <v>3254</v>
+      </c>
+      <c r="J23" s="92">
+        <f>J17*2+J20*2</f>
+        <v>3166</v>
+      </c>
+      <c r="K23" s="92">
+        <f>K17*2+K20*2</f>
+        <v>4384</v>
+      </c>
+      <c r="L23" s="93">
+        <f>L17*2+L20*2</f>
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="94">
+        <f t="shared" ref="C24:F24" si="8">C18*2+C21*2</f>
+        <v>3432</v>
+      </c>
+      <c r="D24" s="94">
+        <f t="shared" si="8"/>
+        <v>3611.3334</v>
+      </c>
+      <c r="E24" s="94">
+        <f t="shared" si="8"/>
+        <v>4419.9333999999999</v>
+      </c>
+      <c r="F24" s="95">
+        <f t="shared" si="8"/>
+        <v>3380.6668</v>
+      </c>
+      <c r="H24" s="100" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="94">
+        <f t="shared" ref="I24:L24" si="9">I18*2+I21*2</f>
+        <v>2907.5</v>
+      </c>
+      <c r="J24" s="94">
+        <f t="shared" si="9"/>
+        <v>2932</v>
+      </c>
+      <c r="K24" s="94">
+        <f t="shared" si="9"/>
+        <v>4036.5</v>
+      </c>
+      <c r="L24" s="95">
+        <f t="shared" si="9"/>
+        <v>4425.1000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="96">
+        <f t="shared" ref="C25:F25" si="10">C19*2+C22*2</f>
+        <v>2898</v>
+      </c>
+      <c r="D25" s="96">
+        <f t="shared" si="10"/>
+        <v>3040</v>
+      </c>
+      <c r="E25" s="96">
+        <f t="shared" si="10"/>
+        <v>4032</v>
+      </c>
+      <c r="F25" s="97">
+        <f t="shared" si="10"/>
+        <v>3882</v>
+      </c>
+      <c r="H25" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="96">
+        <f t="shared" ref="I25:L25" si="11">I19*2+I22*2</f>
+        <v>2614</v>
+      </c>
+      <c r="J25" s="96">
+        <f t="shared" si="11"/>
+        <v>2766</v>
+      </c>
+      <c r="K25" s="96">
+        <f t="shared" si="11"/>
+        <v>3840</v>
+      </c>
+      <c r="L25" s="97">
+        <f t="shared" si="11"/>
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="92">
+        <f>C20*C17</f>
+        <v>912582</v>
+      </c>
+      <c r="D26" s="92">
+        <f>D20*D17</f>
+        <v>980317</v>
+      </c>
+      <c r="E26" s="92">
+        <f>E20*E17</f>
+        <v>1336720</v>
+      </c>
+      <c r="F26" s="93">
+        <f>F20*F17</f>
+        <v>1237390</v>
+      </c>
+      <c r="H26" s="99" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="92">
+        <f>I20*I17</f>
+        <v>658360</v>
+      </c>
+      <c r="J26" s="92">
+        <f>J20*J17</f>
+        <v>622812</v>
+      </c>
+      <c r="K26" s="92">
+        <f>K20*K17</f>
+        <v>1098175</v>
+      </c>
+      <c r="L26" s="93">
+        <f>L20*L17</f>
+        <v>1122548</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="94">
+        <f>C21*C18</f>
+        <v>728995.54991110996</v>
+      </c>
+      <c r="D27" s="94">
+        <f>D21*D18</f>
+        <v>814916.69629999995</v>
+      </c>
+      <c r="E27" s="94">
+        <f>E21*E18</f>
+        <v>1136704.4465099999</v>
+      </c>
+      <c r="F27" s="95">
+        <f>F21*F18</f>
+        <v>700734.50078888994</v>
+      </c>
+      <c r="H27" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="94">
+        <f>I21*I18</f>
+        <v>526079.125</v>
+      </c>
+      <c r="J27" s="94">
+        <f>J21*J18</f>
+        <v>534838.75</v>
+      </c>
+      <c r="K27" s="94">
+        <f>K21*K18</f>
+        <v>922000.625</v>
+      </c>
+      <c r="L27" s="95">
+        <f>L21*L18</f>
+        <v>992459.32499999995</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="96">
+        <f>C22*C19</f>
+        <v>521820</v>
+      </c>
+      <c r="D28" s="96">
+        <f>D22*D19</f>
+        <v>577239</v>
+      </c>
+      <c r="E28" s="96">
+        <f>E22*E19</f>
+        <v>934268</v>
+      </c>
+      <c r="F28" s="97">
+        <f>F22*F19</f>
+        <v>846698</v>
+      </c>
+      <c r="H28" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="96">
+        <f>I22*I19</f>
+        <v>425422</v>
+      </c>
+      <c r="J28" s="96">
+        <f>J22*J19</f>
+        <v>476532</v>
+      </c>
+      <c r="K28" s="96">
+        <f>K22*K19</f>
+        <v>816624</v>
+      </c>
+      <c r="L28" s="97">
+        <f>L22*L19</f>
+        <v>883264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="110" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="111"/>
+      <c r="E2" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="111"/>
+    </row>
+    <row r="3" spans="2:6" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="90">
+        <v>75</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="90">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="89">
+        <v>59</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="89">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="110" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="111"/>
+      <c r="E5" s="110" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="111"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="90">
+        <v>187</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="90">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="43">
+        <v>136</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="43">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="108"/>
+      <c r="E2" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="108"/>
+      <c r="H2" s="107" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="108"/>
+      <c r="K2" s="107" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="108"/>
+    </row>
+    <row r="3" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="90">
+        <v>458116</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="90">
+        <v>885202</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="90">
+        <v>584497</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="90">
+        <v>815131</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="43">
+        <v>420298</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="43">
+        <v>548875</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="43">
+        <v>450796</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="43">
+        <v>614303</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="90">
+        <v>0.50570000000000004</v>
+      </c>
+      <c r="E5" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="105">
+        <v>0.41189999999999999</v>
+      </c>
+      <c r="H5" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="105">
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="K5" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="105">
+        <v>0.41549999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="43">
+        <v>0.38329999999999997</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="43">
+        <v>0.3931</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="43">
+        <v>0.31159999999999999</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="43">
+        <v>0.37940000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="105">
+        <v>25.988900000000001</v>
+      </c>
+      <c r="E7" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="105">
+        <v>39.427199999999999</v>
+      </c>
+      <c r="H7" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="109">
+        <v>28</v>
+      </c>
+      <c r="K7" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="105">
+        <v>24.293800000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="43">
+        <v>23.2623</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="106">
+        <v>37.735500000000002</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="43">
+        <v>24.7956</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="43">
+        <v>22.673400000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="103">
+        <v>770016</v>
+      </c>
+      <c r="D9" s="102"/>
+      <c r="E9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="103">
+        <v>1476860</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="103">
+        <v>875465</v>
+      </c>
+      <c r="J9" s="102"/>
+      <c r="K9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="103">
+        <v>1122548</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="43">
+        <v>624624</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="43">
+        <v>1063834</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="43">
+        <v>630198</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="43">
+        <v>883264</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:12" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:W13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="H2" s="117" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="O2" s="117" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="116">
+        <v>4.8986486486486486E-2</v>
+      </c>
+      <c r="F3" s="116"/>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="116">
+        <v>0.12821534671400622</v>
+      </c>
+      <c r="M3" s="116"/>
+      <c r="O3" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="116">
+        <v>0.25799313643651206</v>
+      </c>
+      <c r="T3" s="116"/>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="116">
+        <v>0.14954682779456194</v>
+      </c>
+      <c r="F4" s="116"/>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="116">
+        <v>8.8297496558220421E-3</v>
+      </c>
+      <c r="M4" s="116"/>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="116">
+        <v>2.0237461485102168E-2</v>
+      </c>
+      <c r="T4" s="116"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="116">
+        <v>6.0422960725075529E-3</v>
+      </c>
+      <c r="F5" s="116"/>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="116">
+        <v>0.17706615881801108</v>
+      </c>
+      <c r="M5" s="116"/>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="116">
+        <v>0.35620834492719056</v>
+      </c>
+      <c r="T5" s="116"/>
+      <c r="U5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="L6" s="116"/>
+      <c r="M6" s="116"/>
+      <c r="S6" s="116"/>
+      <c r="T6" s="116"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="117" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="117"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="117"/>
+      <c r="H8" s="117" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="117"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="117"/>
+      <c r="L8" s="117"/>
+      <c r="O8" s="117" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" s="117"/>
+      <c r="Q8" s="117"/>
+      <c r="R8" s="117"/>
+      <c r="S8" s="117"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="116">
+        <v>0.14142091152815014</v>
+      </c>
+      <c r="F9" s="116"/>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="116">
+        <v>0.25425075247882561</v>
+      </c>
+      <c r="M9" s="116"/>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S9" s="116">
+        <v>5.5309157318027651E-2</v>
+      </c>
+      <c r="T9" s="116"/>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="116">
+        <v>4.2600896860986545E-2</v>
+      </c>
+      <c r="F10" s="116"/>
+      <c r="H10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="116">
+        <v>4.8520030017759966E-2</v>
+      </c>
+      <c r="M10" s="116"/>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>68</v>
+      </c>
+      <c r="S10" s="116">
+        <v>4.5598313125988499E-2</v>
+      </c>
+      <c r="T10" s="116"/>
+      <c r="W10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="116"/>
+      <c r="F11" s="116"/>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="116"/>
+      <c r="M11" s="116"/>
+      <c r="O11" t="s">
+        <v>70</v>
+      </c>
+      <c r="S11" s="116">
+        <v>7.8860340880183233E-2</v>
+      </c>
+      <c r="T11" s="116"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" t="s">
+        <v>65</v>
+      </c>
+      <c r="S12" s="116"/>
+      <c r="T12" s="116"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" s="116">
+        <v>0.15734336312861893</v>
+      </c>
+      <c r="M13" s="116"/>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="T13" s="116">
+        <v>1.7396004913556524E-4</v>
+      </c>
+      <c r="U13" s="116">
+        <v>2.8538765940276833E-2</v>
+      </c>
+      <c r="V13" s="116">
+        <v>1.0998410216632227E-4</v>
+      </c>
+      <c r="W13" s="116">
+        <v>2.9910190273301335E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>